<commit_message>
Change Belage_tidy.csv and Change "Gewichtung" for Belaege_Gwichtung_Szenario 0 to 3.csv
</commit_message>
<xml_diff>
--- a/00_data_raw/Rohdaten_Matrix_Baeume.xlsx
+++ b/00_data_raw/Rohdaten_Matrix_Baeume.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zhaw-my.sharepoint.com/personal/pfeifsar_students_zhaw_ch/Documents/6. Semester MSc UnR/Thesis/R_Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zhaw-my.sharepoint.com/personal/pfeifsar_students_zhaw_ch/Documents/6. Semester MSc UnR/Thesis/R_Project/00_data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{F5B91F4B-6C5E-40FC-8FE7-21E477E3C12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7767779D-7327-419A-B72D-A8A9706F3217}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{F5B91F4B-6C5E-40FC-8FE7-21E477E3C12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4B7E905-A649-4AC5-873A-42AF3C1E32A9}"/>
   <bookViews>
-    <workbookView xWindow="-19305" yWindow="-1350" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rohdaten_Matrix_Baeume" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="84">
   <si>
     <t>Baumkategorie</t>
   </si>
@@ -292,6 +292,15 @@
 Mittelgrosse Arten: 150–250 l H₂O/Tag
 Kleine Arten: 80–150 l H₂O/Tag
 Diese Spanne berücksichtigt sowohl Transpiration als auch Interzeption (Niederschlagsrückhalt auf der Krone).</t>
+  </si>
+  <si>
+    <t>Recyclingpotential</t>
+  </si>
+  <si>
+    <t>Das Recycling- bzw. Wiederverwendungspotenzial der Baumarten wurde auf Grundlage von Schwedt (2021) in drei Stufen bewertet:
+hoch (3) steht für langlebige stoffliche Anwendungen wie Bauholz, Möbel oder Parkett, bei denen das Holz über viele Jahre im Nutzungskreislauf verbleibt;
+mittel (2) beschreibt begrenzte stoffliche Nutzungen wie Innenverkleidung, Blind- oder Schnitzholz;
+gering (1) kennzeichnet kurzlebige oder überwiegend energetische Verwendungen, etwa als Brennholz, Papier- oder Verpackungsmaterial.</t>
   </si>
 </sst>
 </file>
@@ -347,12 +356,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -367,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -407,6 +422,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -422,6 +449,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -627,8 +658,8 @@
   </sheetPr>
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -645,7 +676,7 @@
     <col min="10" max="10" width="45.08984375" customWidth="1"/>
     <col min="11" max="11" width="22.6328125" customWidth="1"/>
     <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="225.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="5" customFormat="1" ht="15.5" customHeight="1">
@@ -685,7 +716,9 @@
       <c r="L1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="4"/>
+      <c r="M1" s="4" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -724,7 +757,9 @@
       <c r="L2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="6"/>
+      <c r="M2" s="9" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="3" spans="1:13" ht="15.5" customHeight="1">
       <c r="A3" s="2" t="s">
@@ -763,7 +798,9 @@
       <c r="L3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="6"/>
+      <c r="M3" s="9" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
@@ -802,7 +839,9 @@
       <c r="L4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="M4" s="7"/>
+      <c r="M4" s="17" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
@@ -841,7 +880,9 @@
       <c r="L5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="M5" s="6"/>
+      <c r="M5" s="9" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
@@ -880,7 +921,9 @@
       <c r="L6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M6" s="6"/>
+      <c r="M6" s="9" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="7" spans="1:13" ht="15.5" customHeight="1">
       <c r="A7" s="2" t="s">
@@ -919,7 +962,9 @@
       <c r="L7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="M7" s="6"/>
+      <c r="M7" s="18" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1">
       <c r="A8" s="2" t="s">
@@ -958,7 +1003,9 @@
       <c r="L8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M8" s="7"/>
+      <c r="M8" s="17" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1">
       <c r="A9" s="2" t="s">
@@ -997,7 +1044,9 @@
       <c r="L9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="M9" s="7"/>
+      <c r="M9" s="17" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
@@ -1036,7 +1085,9 @@
       <c r="L10" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="M10" s="6"/>
+      <c r="M10" s="18" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
@@ -1075,7 +1126,9 @@
       <c r="L11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="M11" s="6"/>
+      <c r="M11" s="9" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1">
       <c r="A12" s="3" t="s">
@@ -1114,7 +1167,9 @@
       <c r="L12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="M12" s="7"/>
+      <c r="M12" s="19" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="13" spans="1:13" ht="12.5">
       <c r="A13" s="3" t="s">
@@ -1153,7 +1208,9 @@
       <c r="L13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="M13" s="7"/>
+      <c r="M13" s="19" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="14" spans="1:13" ht="15.75" customHeight="1">
       <c r="A14" s="1" t="s">
@@ -1192,7 +1249,9 @@
       <c r="L14" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="M14" s="6"/>
+      <c r="M14" s="18" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
       <c r="A15" s="3" t="s">
@@ -1231,7 +1290,9 @@
       <c r="L15" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="M15" s="6"/>
+      <c r="M15" s="18" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1">
       <c r="A16" s="3" t="s">
@@ -1270,7 +1331,9 @@
       <c r="L16" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="M16" s="6"/>
+      <c r="M16" s="18" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
@@ -1309,7 +1372,9 @@
       <c r="L17" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="M17" s="6"/>
+      <c r="M17" s="18" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1">
       <c r="A18" s="3" t="s">
@@ -1348,7 +1413,9 @@
       <c r="L18" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="M18" s="7"/>
+      <c r="M18" s="19" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="21" spans="1:13" ht="27" customHeight="1">
       <c r="A21" s="16" t="s">
@@ -1435,7 +1502,14 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="12.5"/>
+    <row r="32" spans="1:13" ht="153.5" customHeight="1">
+      <c r="A32" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>83</v>
+      </c>
+    </row>
     <row r="33" spans="1:5" ht="13">
       <c r="A33" s="14"/>
       <c r="B33" s="13"/>

</xml_diff>

<commit_message>
Code "MCA Baeume" verified and fixes
</commit_message>
<xml_diff>
--- a/00_data_raw/Rohdaten_Matrix_Baeume.xlsx
+++ b/00_data_raw/Rohdaten_Matrix_Baeume.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zhaw-my.sharepoint.com/personal/pfeifsar_students_zhaw_ch/Documents/6. Semester MSc UnR/Thesis/R_Project/00_data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="686" documentId="13_ncr:1_{F5B91F4B-6C5E-40FC-8FE7-21E477E3C12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C941893-44BB-416D-BBAF-70087F69C8FF}"/>
+  <xr:revisionPtr revIDLastSave="704" documentId="13_ncr:1_{F5B91F4B-6C5E-40FC-8FE7-21E477E3C12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F705F42-DEA2-47B2-8E8B-3FC7277FC958}"/>
   <bookViews>
-    <workbookView xWindow="-19305" yWindow="-1350" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rohdaten_Baeume" sheetId="1" r:id="rId1"/>
@@ -855,8 +855,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -903,6 +901,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1127,8 +1127,8 @@
   </sheetPr>
   <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="H14" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2:R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1143,77 +1143,77 @@
     <col min="8" max="8" width="25.90625" customWidth="1"/>
     <col min="9" max="9" width="31.08984375" customWidth="1"/>
     <col min="10" max="10" width="21.54296875" customWidth="1"/>
-    <col min="11" max="11" width="23.08984375" customWidth="1"/>
-    <col min="12" max="12" width="14.453125" customWidth="1"/>
-    <col min="13" max="13" width="17.90625" customWidth="1"/>
-    <col min="14" max="14" width="22.1796875" customWidth="1"/>
-    <col min="15" max="15" width="25.90625" customWidth="1"/>
-    <col min="16" max="16" width="28.54296875" customWidth="1"/>
-    <col min="17" max="17" width="30.90625" customWidth="1"/>
+    <col min="11" max="11" width="23.08984375" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.453125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="17.90625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="22.1796875" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="25.90625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="28.54296875" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="30.90625" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="22.6328125" customWidth="1"/>
     <col min="19" max="19" width="18.26953125" customWidth="1"/>
     <col min="20" max="20" width="22.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="5" customFormat="1" ht="15.5" customHeight="1">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:20" s="23" customFormat="1" ht="15.5" customHeight="1">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="22" t="s">
         <v>120</v>
       </c>
     </row>
@@ -1221,66 +1221,66 @@
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="9">
+      <c r="E2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="7">
         <f>AVERAGE(80,120)</f>
         <v>100</v>
       </c>
-      <c r="G2" s="9">
-        <v>2</v>
-      </c>
-      <c r="H2" s="9">
+      <c r="G2" s="7">
+        <v>2</v>
+      </c>
+      <c r="H2" s="7">
         <v>1</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="9">
+      <c r="J2" s="7">
         <f>AVERAGE(15,20)</f>
         <v>17.5</v>
       </c>
-      <c r="K2" s="9">
+      <c r="K2" s="7">
         <v>4.7</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="22">
+      <c r="M2" s="20">
         <f>AVERAGE(4,6)</f>
         <v>5</v>
       </c>
-      <c r="N2" s="9">
+      <c r="N2" s="7">
         <v>50</v>
       </c>
-      <c r="O2" s="9">
+      <c r="O2" s="7">
         <f>N2</f>
         <v>50</v>
       </c>
-      <c r="P2" s="10" t="s">
+      <c r="P2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="Q2" s="10">
+      <c r="Q2" s="8">
         <f>AVERAGE(250,400)</f>
         <v>325</v>
       </c>
-      <c r="R2" s="9">
+      <c r="R2" s="7">
         <v>38</v>
       </c>
-      <c r="S2" s="9">
-        <v>2</v>
-      </c>
-      <c r="T2" s="9">
+      <c r="S2" s="7">
+        <v>2</v>
+      </c>
+      <c r="T2" s="7">
         <v>3</v>
       </c>
     </row>
@@ -1288,66 +1288,66 @@
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="9">
+      <c r="E3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="7">
         <f>AVERAGE(80,120)</f>
         <v>100</v>
       </c>
-      <c r="G3" s="9">
-        <v>2</v>
-      </c>
-      <c r="H3" s="9">
-        <v>2</v>
-      </c>
-      <c r="I3" s="9" t="s">
+      <c r="G3" s="7">
+        <v>2</v>
+      </c>
+      <c r="H3" s="7">
+        <v>2</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="9">
+      <c r="J3" s="7">
         <f t="shared" ref="J3:J4" si="0">AVERAGE(15,20)</f>
         <v>17.5</v>
       </c>
-      <c r="K3" s="9">
+      <c r="K3" s="7">
         <v>4.4000000000000004</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="L3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="22">
+      <c r="M3" s="20">
         <f t="shared" ref="M3:M7" si="1">AVERAGE(4,6)</f>
         <v>5</v>
       </c>
-      <c r="N3" s="9">
+      <c r="N3" s="7">
         <v>50</v>
       </c>
-      <c r="O3" s="9">
+      <c r="O3" s="7">
         <f t="shared" ref="O3:O7" si="2">N3</f>
         <v>50</v>
       </c>
-      <c r="P3" s="10" t="s">
+      <c r="P3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="Q3" s="10">
+      <c r="Q3" s="8">
         <f t="shared" ref="Q3:Q7" si="3">AVERAGE(250,400)</f>
         <v>325</v>
       </c>
-      <c r="R3" s="9">
+      <c r="R3" s="7">
         <v>38</v>
       </c>
-      <c r="S3" s="9">
-        <v>2</v>
-      </c>
-      <c r="T3" s="9">
+      <c r="S3" s="7">
+        <v>2</v>
+      </c>
+      <c r="T3" s="7">
         <v>3</v>
       </c>
     </row>
@@ -1355,66 +1355,66 @@
       <c r="A4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="7">
         <f>AVERAGE(70,90)</f>
         <v>80</v>
       </c>
-      <c r="G4" s="9">
-        <v>3</v>
-      </c>
-      <c r="H4" s="9">
-        <v>3</v>
-      </c>
-      <c r="I4" s="9" t="s">
+      <c r="G4" s="7">
+        <v>3</v>
+      </c>
+      <c r="H4" s="7">
+        <v>3</v>
+      </c>
+      <c r="I4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="7">
         <f t="shared" si="0"/>
         <v>17.5</v>
       </c>
-      <c r="K4" s="8">
+      <c r="K4" s="6">
         <v>3.6</v>
       </c>
-      <c r="L4" s="15" t="s">
+      <c r="L4" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="M4" s="22">
+      <c r="M4" s="20">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="N4" s="9">
+      <c r="N4" s="7">
         <v>50</v>
       </c>
-      <c r="O4" s="9">
+      <c r="O4" s="7">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="P4" s="10" t="s">
+      <c r="P4" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="Q4" s="10">
+      <c r="Q4" s="8">
         <f t="shared" si="3"/>
         <v>325</v>
       </c>
-      <c r="R4" s="9">
+      <c r="R4" s="7">
         <v>38</v>
       </c>
-      <c r="S4" s="9">
-        <v>3</v>
-      </c>
-      <c r="T4" s="23">
+      <c r="S4" s="7">
+        <v>3</v>
+      </c>
+      <c r="T4" s="21">
         <v>2</v>
       </c>
     </row>
@@ -1422,66 +1422,66 @@
       <c r="A5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="9">
+      <c r="E5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="7">
         <f>AVERAGE(60,100)</f>
         <v>80</v>
       </c>
-      <c r="G5" s="9">
-        <v>2</v>
-      </c>
-      <c r="H5" s="9">
-        <v>3</v>
-      </c>
-      <c r="I5" s="15" t="s">
+      <c r="G5" s="7">
+        <v>2</v>
+      </c>
+      <c r="H5" s="7">
+        <v>3</v>
+      </c>
+      <c r="I5" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="7">
         <f>AVERAGE(12,15)</f>
         <v>13.5</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="6">
         <v>4.4000000000000004</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="L5" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="M5" s="22">
+      <c r="M5" s="20">
         <f>AVERAGE(2,4)</f>
         <v>3</v>
       </c>
-      <c r="N5" s="9" t="s">
+      <c r="N5" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="O5" s="9">
+      <c r="O5" s="7">
         <f>AVERAGE(30,45)</f>
         <v>37.5</v>
       </c>
-      <c r="P5" s="10" t="s">
+      <c r="P5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="Q5" s="10">
+      <c r="Q5" s="8">
         <f>AVERAGE(150,250)</f>
         <v>200</v>
       </c>
-      <c r="R5" s="9">
+      <c r="R5" s="7">
         <v>38</v>
       </c>
-      <c r="S5" s="9">
-        <v>3</v>
-      </c>
-      <c r="T5" s="9">
+      <c r="S5" s="7">
+        <v>3</v>
+      </c>
+      <c r="T5" s="7">
         <v>2</v>
       </c>
     </row>
@@ -1489,66 +1489,66 @@
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="9">
+      <c r="E6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="7">
         <f>AVERAGE(80,120)</f>
         <v>100</v>
       </c>
-      <c r="G6" s="9">
-        <v>2</v>
-      </c>
-      <c r="H6" s="9">
-        <v>3</v>
-      </c>
-      <c r="I6" s="15" t="s">
+      <c r="G6" s="7">
+        <v>2</v>
+      </c>
+      <c r="H6" s="7">
+        <v>3</v>
+      </c>
+      <c r="I6" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="7">
         <f>AVERAGE(12,18)</f>
         <v>15</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="7">
         <v>4</v>
       </c>
-      <c r="L6" s="15" t="s">
+      <c r="L6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="M6" s="22">
+      <c r="M6" s="20">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="N6" s="9">
+      <c r="N6" s="7">
         <v>50</v>
       </c>
-      <c r="O6" s="9">
+      <c r="O6" s="7">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="P6" s="10" t="s">
+      <c r="P6" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="Q6" s="10">
+      <c r="Q6" s="8">
         <f t="shared" si="3"/>
         <v>325</v>
       </c>
-      <c r="R6" s="9">
+      <c r="R6" s="7">
         <v>38</v>
       </c>
-      <c r="S6" s="9">
-        <v>2</v>
-      </c>
-      <c r="T6" s="9">
+      <c r="S6" s="7">
+        <v>2</v>
+      </c>
+      <c r="T6" s="7">
         <v>2</v>
       </c>
     </row>
@@ -1556,66 +1556,66 @@
       <c r="A7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="9">
+      <c r="E7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="7">
         <f>AVERAGE(60,100)</f>
         <v>80</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="7">
         <v>1</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="7">
         <v>1</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="I7" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="7">
         <f>AVERAGE(12,18)</f>
         <v>15</v>
       </c>
-      <c r="K7" s="9">
-        <v>2</v>
-      </c>
-      <c r="L7" s="15" t="s">
+      <c r="K7" s="7">
+        <v>2</v>
+      </c>
+      <c r="L7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="M7" s="22">
+      <c r="M7" s="20">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="N7" s="9">
+      <c r="N7" s="7">
         <v>50</v>
       </c>
-      <c r="O7" s="9">
+      <c r="O7" s="7">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="P7" s="10" t="s">
+      <c r="P7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="Q7" s="10">
+      <c r="Q7" s="8">
         <f t="shared" si="3"/>
         <v>325</v>
       </c>
-      <c r="R7" s="9">
+      <c r="R7" s="7">
         <v>38</v>
       </c>
-      <c r="S7" s="9">
-        <v>2</v>
-      </c>
-      <c r="T7" s="9">
+      <c r="S7" s="7">
+        <v>2</v>
+      </c>
+      <c r="T7" s="7">
         <v>2</v>
       </c>
     </row>
@@ -1623,66 +1623,66 @@
       <c r="A8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="7">
         <f>AVERAGE(60,80)</f>
         <v>70</v>
       </c>
-      <c r="G8" s="9">
-        <v>2</v>
-      </c>
-      <c r="H8" s="9">
+      <c r="G8" s="7">
+        <v>2</v>
+      </c>
+      <c r="H8" s="7">
         <v>1</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="I8" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="9">
+      <c r="J8" s="7">
         <f>AVERAGE(8,10)</f>
         <v>9</v>
       </c>
-      <c r="K8" s="9">
+      <c r="K8" s="7">
         <v>1.4</v>
       </c>
-      <c r="L8" s="15" t="s">
+      <c r="L8" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="M8" s="22">
+      <c r="M8" s="20">
         <f>AVERAGE(2,4)</f>
         <v>3</v>
       </c>
-      <c r="N8" s="9" t="s">
+      <c r="N8" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="O8" s="9">
+      <c r="O8" s="7">
         <f>AVERAGE(30,45)</f>
         <v>37.5</v>
       </c>
-      <c r="P8" s="10" t="s">
+      <c r="P8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="Q8" s="10">
+      <c r="Q8" s="8">
         <f>AVERAGE(120,250)</f>
         <v>185</v>
       </c>
-      <c r="R8" s="9">
+      <c r="R8" s="7">
         <v>24</v>
       </c>
-      <c r="S8" s="9">
-        <v>3</v>
-      </c>
-      <c r="T8" s="9">
+      <c r="S8" s="7">
+        <v>3</v>
+      </c>
+      <c r="T8" s="7">
         <v>2</v>
       </c>
     </row>
@@ -1690,66 +1690,66 @@
       <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="7">
         <f>AVERAGE(60,90)</f>
         <v>75</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="7">
         <v>1</v>
       </c>
-      <c r="H9" s="9">
-        <v>2</v>
-      </c>
-      <c r="I9" s="15" t="s">
+      <c r="H9" s="7">
+        <v>2</v>
+      </c>
+      <c r="I9" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9" s="7">
         <f>AVERAGE(5,8)</f>
         <v>6.5</v>
       </c>
-      <c r="K9" s="9">
-        <v>3</v>
-      </c>
-      <c r="L9" s="15" t="s">
+      <c r="K9" s="7">
+        <v>3</v>
+      </c>
+      <c r="L9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="M9" s="22">
+      <c r="M9" s="20">
         <f t="shared" ref="M9:M16" si="4">AVERAGE(2,4)</f>
         <v>3</v>
       </c>
-      <c r="N9" s="9" t="s">
+      <c r="N9" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="O9" s="9">
+      <c r="O9" s="7">
         <f>AVERAGE(30,45)</f>
         <v>37.5</v>
       </c>
-      <c r="P9" s="10" t="s">
+      <c r="P9" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="Q9" s="10">
+      <c r="Q9" s="8">
         <f>AVERAGE(150,250)</f>
         <v>200</v>
       </c>
-      <c r="R9" s="9">
-        <v>24</v>
-      </c>
-      <c r="S9" s="9">
-        <v>3</v>
-      </c>
-      <c r="T9" s="9">
+      <c r="R9" s="7">
+        <v>13</v>
+      </c>
+      <c r="S9" s="7">
+        <v>3</v>
+      </c>
+      <c r="T9" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1757,66 +1757,66 @@
       <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="9">
+      <c r="E10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="7">
         <f t="shared" ref="F10" si="5">AVERAGE(80,120)</f>
         <v>100</v>
       </c>
-      <c r="G10" s="9">
-        <v>2</v>
-      </c>
-      <c r="H10" s="9">
-        <v>3</v>
-      </c>
-      <c r="I10" s="15" t="s">
+      <c r="G10" s="7">
+        <v>2</v>
+      </c>
+      <c r="H10" s="7">
+        <v>3</v>
+      </c>
+      <c r="I10" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10" s="7">
         <f>AVERAGE(10,15)</f>
         <v>12.5</v>
       </c>
-      <c r="K10" s="9">
+      <c r="K10" s="7">
         <v>2.5</v>
       </c>
-      <c r="L10" s="15" t="s">
+      <c r="L10" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="M10" s="22">
+      <c r="M10" s="20">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="N10" s="9" t="s">
+      <c r="N10" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="O10" s="9">
+      <c r="O10" s="7">
         <f>AVERAGE(30,45)</f>
         <v>37.5</v>
       </c>
-      <c r="P10" s="10" t="s">
+      <c r="P10" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="Q10" s="10">
+      <c r="Q10" s="8">
         <f>AVERAGE(150,250)</f>
         <v>200</v>
       </c>
-      <c r="R10" s="9">
-        <v>24</v>
-      </c>
-      <c r="S10" s="9">
-        <v>3</v>
-      </c>
-      <c r="T10" s="9">
+      <c r="R10" s="7">
+        <v>38</v>
+      </c>
+      <c r="S10" s="7">
+        <v>3</v>
+      </c>
+      <c r="T10" s="7">
         <v>3</v>
       </c>
     </row>
@@ -1824,66 +1824,66 @@
       <c r="A11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="9">
+      <c r="E11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="7">
         <f>AVERAGE(60,100)</f>
         <v>80</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="7">
         <v>1</v>
       </c>
-      <c r="H11" s="9">
-        <v>2</v>
-      </c>
-      <c r="I11" s="15" t="s">
+      <c r="H11" s="7">
+        <v>2</v>
+      </c>
+      <c r="I11" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="7">
         <f>AVERAGE(8,12)</f>
         <v>10</v>
       </c>
-      <c r="K11" s="9">
+      <c r="K11" s="7">
         <v>2.4</v>
       </c>
-      <c r="L11" s="15" t="s">
+      <c r="L11" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="M11" s="22">
+      <c r="M11" s="20">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="N11" s="9" t="s">
+      <c r="N11" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="O11" s="9">
+      <c r="O11" s="7">
         <f>AVERAGE(30,45)</f>
         <v>37.5</v>
       </c>
-      <c r="P11" s="10" t="s">
+      <c r="P11" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="Q11" s="10">
+      <c r="Q11" s="8">
         <f>AVERAGE(150,250)</f>
         <v>200</v>
       </c>
-      <c r="R11" s="9">
+      <c r="R11" s="7">
         <v>24</v>
       </c>
-      <c r="S11" s="9">
-        <v>2</v>
-      </c>
-      <c r="T11" s="9">
+      <c r="S11" s="7">
+        <v>2</v>
+      </c>
+      <c r="T11" s="7">
         <v>2</v>
       </c>
     </row>
@@ -1891,66 +1891,66 @@
       <c r="A12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="9">
+      <c r="E12" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="7">
         <f>AVERAGE(60,100)</f>
         <v>80</v>
       </c>
-      <c r="G12" s="9">
-        <v>2</v>
-      </c>
-      <c r="H12" s="9">
-        <v>2</v>
-      </c>
-      <c r="I12" s="15" t="s">
+      <c r="G12" s="7">
+        <v>2</v>
+      </c>
+      <c r="H12" s="7">
+        <v>2</v>
+      </c>
+      <c r="I12" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="J12" s="9">
+      <c r="J12" s="7">
         <f>AVERAGE(6,10)</f>
         <v>8</v>
       </c>
-      <c r="K12" s="9">
-        <v>2</v>
-      </c>
-      <c r="L12" s="15" t="s">
+      <c r="K12" s="7">
+        <v>2</v>
+      </c>
+      <c r="L12" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="M12" s="22">
+      <c r="M12" s="20">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="N12" s="9" t="s">
+      <c r="N12" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="O12" s="9">
+      <c r="O12" s="7">
         <f>AVERAGE(30,45)</f>
         <v>37.5</v>
       </c>
-      <c r="P12" s="10" t="s">
+      <c r="P12" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="Q12" s="10">
+      <c r="Q12" s="8">
         <f>AVERAGE(150,250)</f>
         <v>200</v>
       </c>
-      <c r="R12" s="9">
+      <c r="R12" s="7">
         <v>24</v>
       </c>
-      <c r="S12" s="9">
-        <v>3</v>
-      </c>
-      <c r="T12" s="9">
+      <c r="S12" s="7">
+        <v>3</v>
+      </c>
+      <c r="T12" s="7">
         <v>3</v>
       </c>
     </row>
@@ -1958,66 +1958,66 @@
       <c r="A13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="9">
+      <c r="E13" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="7">
         <f>AVERAGE(80,120)</f>
         <v>100</v>
       </c>
-      <c r="G13" s="9">
-        <v>3</v>
-      </c>
-      <c r="H13" s="9">
-        <v>3</v>
-      </c>
-      <c r="I13" s="15" t="s">
+      <c r="G13" s="7">
+        <v>3</v>
+      </c>
+      <c r="H13" s="7">
+        <v>3</v>
+      </c>
+      <c r="I13" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13" s="7">
         <f>AVERAGE(5,6)</f>
         <v>5.5</v>
       </c>
-      <c r="K13" s="8">
+      <c r="K13" s="6">
         <v>2.2999999999999998</v>
       </c>
-      <c r="L13" s="15" t="s">
+      <c r="L13" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="M13" s="22">
+      <c r="M13" s="20">
         <f>AVERAGE(1,2)</f>
         <v>1.5</v>
       </c>
-      <c r="N13" s="9" t="s">
+      <c r="N13" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="O13" s="9">
+      <c r="O13" s="7">
         <f>AVERAGE(20,35)</f>
         <v>27.5</v>
       </c>
-      <c r="P13" s="10" t="s">
+      <c r="P13" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="Q13" s="10">
+      <c r="Q13" s="8">
         <f>AVERAGE(80,150)</f>
         <v>115</v>
       </c>
-      <c r="R13" s="9">
+      <c r="R13" s="7">
         <v>13</v>
       </c>
-      <c r="S13" s="9">
-        <v>2</v>
-      </c>
-      <c r="T13" s="23">
+      <c r="S13" s="7">
+        <v>2</v>
+      </c>
+      <c r="T13" s="21">
         <v>3</v>
       </c>
     </row>
@@ -2025,66 +2025,66 @@
       <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="9">
+      <c r="E14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="7">
         <f>AVERAGE(60,100)</f>
         <v>80</v>
       </c>
-      <c r="G14" s="9">
-        <v>3</v>
-      </c>
-      <c r="H14" s="9">
-        <v>3</v>
-      </c>
-      <c r="I14" s="15" t="s">
+      <c r="G14" s="7">
+        <v>3</v>
+      </c>
+      <c r="H14" s="7">
+        <v>3</v>
+      </c>
+      <c r="I14" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J14" s="7">
         <f>AVERAGE(4,6)</f>
         <v>5</v>
       </c>
-      <c r="K14" s="8">
+      <c r="K14" s="6">
         <v>4.3</v>
       </c>
-      <c r="L14" s="15" t="s">
+      <c r="L14" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="M14" s="22">
+      <c r="M14" s="20">
         <f>AVERAGE(1,2)</f>
         <v>1.5</v>
       </c>
-      <c r="N14" s="9" t="s">
+      <c r="N14" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="O14" s="9">
+      <c r="O14" s="7">
         <f>AVERAGE(20,35)</f>
         <v>27.5</v>
       </c>
-      <c r="P14" s="10" t="s">
+      <c r="P14" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="Q14" s="10">
+      <c r="Q14" s="8">
         <f>AVERAGE(80,150)</f>
         <v>115</v>
       </c>
-      <c r="R14" s="9">
+      <c r="R14" s="7">
         <v>13</v>
       </c>
-      <c r="S14" s="9">
-        <v>3</v>
-      </c>
-      <c r="T14" s="23">
+      <c r="S14" s="7">
+        <v>3</v>
+      </c>
+      <c r="T14" s="21">
         <v>2</v>
       </c>
     </row>
@@ -2092,66 +2092,66 @@
       <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="7">
         <f>AVERAGE(70,100)</f>
         <v>85</v>
       </c>
-      <c r="G15" s="9">
-        <v>3</v>
-      </c>
-      <c r="H15" s="9">
-        <v>2</v>
-      </c>
-      <c r="I15" s="15" t="s">
+      <c r="G15" s="7">
+        <v>3</v>
+      </c>
+      <c r="H15" s="7">
+        <v>2</v>
+      </c>
+      <c r="I15" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J15" s="7">
         <f>AVERAGE(10,15)</f>
         <v>12.5</v>
       </c>
-      <c r="K15" s="9">
+      <c r="K15" s="7">
         <v>2.2000000000000002</v>
       </c>
-      <c r="L15" s="15" t="s">
+      <c r="L15" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="M15" s="22">
+      <c r="M15" s="20">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="N15" s="9" t="s">
+      <c r="N15" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="O15" s="9">
+      <c r="O15" s="7">
         <f>AVERAGE(30,45)</f>
         <v>37.5</v>
       </c>
-      <c r="P15" s="10" t="s">
+      <c r="P15" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="Q15" s="10">
+      <c r="Q15" s="8">
         <f>AVERAGE(150,250)</f>
         <v>200</v>
       </c>
-      <c r="R15" s="9">
+      <c r="R15" s="7">
         <v>38</v>
       </c>
-      <c r="S15" s="9">
-        <v>3</v>
-      </c>
-      <c r="T15" s="9">
+      <c r="S15" s="7">
+        <v>3</v>
+      </c>
+      <c r="T15" s="7">
         <v>2</v>
       </c>
     </row>
@@ -2159,66 +2159,66 @@
       <c r="A16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F16" s="9">
+      <c r="E16" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="7">
         <f>AVERAGE(60,100)</f>
         <v>80</v>
       </c>
-      <c r="G16" s="9">
-        <v>3</v>
-      </c>
-      <c r="H16" s="9">
-        <v>3</v>
-      </c>
-      <c r="I16" s="15" t="s">
+      <c r="G16" s="7">
+        <v>3</v>
+      </c>
+      <c r="H16" s="7">
+        <v>3</v>
+      </c>
+      <c r="I16" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="J16" s="9">
+      <c r="J16" s="7">
         <f>AVERAGE(8,12)</f>
         <v>10</v>
       </c>
-      <c r="K16" s="9">
+      <c r="K16" s="7">
         <v>2.4</v>
       </c>
-      <c r="L16" s="15" t="s">
+      <c r="L16" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="M16" s="22">
+      <c r="M16" s="20">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="N16" s="9" t="s">
+      <c r="N16" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="O16" s="9">
+      <c r="O16" s="7">
         <f>AVERAGE(30,45)</f>
         <v>37.5</v>
       </c>
-      <c r="P16" s="10" t="s">
+      <c r="P16" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="Q16" s="10">
+      <c r="Q16" s="8">
         <f>AVERAGE(150,250)</f>
         <v>200</v>
       </c>
-      <c r="R16" s="9">
+      <c r="R16" s="7">
         <v>24</v>
       </c>
-      <c r="S16" s="9">
-        <v>3</v>
-      </c>
-      <c r="T16" s="9">
+      <c r="S16" s="7">
+        <v>3</v>
+      </c>
+      <c r="T16" s="7">
         <v>3</v>
       </c>
     </row>
@@ -2226,66 +2226,66 @@
       <c r="A17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="7">
         <f>AVERAGE(60,90)</f>
         <v>75</v>
       </c>
-      <c r="G17" s="9">
-        <v>2</v>
-      </c>
-      <c r="H17" s="9">
-        <v>3</v>
-      </c>
-      <c r="I17" s="15" t="s">
+      <c r="G17" s="7">
+        <v>2</v>
+      </c>
+      <c r="H17" s="7">
+        <v>3</v>
+      </c>
+      <c r="I17" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="J17" s="9">
+      <c r="J17" s="7">
         <f>AVERAGE(4,7)</f>
         <v>5.5</v>
       </c>
-      <c r="K17" s="9">
+      <c r="K17" s="7">
         <v>4.0999999999999996</v>
       </c>
-      <c r="L17" s="15" t="s">
+      <c r="L17" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="M17" s="22">
+      <c r="M17" s="20">
         <f>AVERAGE(1,2)</f>
         <v>1.5</v>
       </c>
-      <c r="N17" s="9" t="s">
+      <c r="N17" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="O17" s="9">
+      <c r="O17" s="7">
         <f>AVERAGE(20,35)</f>
         <v>27.5</v>
       </c>
-      <c r="P17" s="9" t="s">
+      <c r="P17" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Q17" s="10">
+      <c r="Q17" s="8">
         <f>AVERAGE(80,150)</f>
         <v>115</v>
       </c>
-      <c r="R17" s="9">
+      <c r="R17" s="7">
         <v>13</v>
       </c>
-      <c r="S17" s="9">
-        <v>3</v>
-      </c>
-      <c r="T17" s="23">
+      <c r="S17" s="7">
+        <v>3</v>
+      </c>
+      <c r="T17" s="21">
         <v>2</v>
       </c>
     </row>
@@ -2293,66 +2293,66 @@
       <c r="A18" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="7">
         <f>AVERAGE(70,100)</f>
         <v>85</v>
       </c>
-      <c r="G18" s="9">
-        <v>2</v>
-      </c>
-      <c r="H18" s="9">
-        <v>2</v>
-      </c>
-      <c r="I18" s="15" t="s">
+      <c r="G18" s="7">
+        <v>2</v>
+      </c>
+      <c r="H18" s="7">
+        <v>2</v>
+      </c>
+      <c r="I18" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J18" s="9">
+      <c r="J18" s="7">
         <f>AVERAGE(4,6)</f>
         <v>5</v>
       </c>
-      <c r="K18" s="9">
+      <c r="K18" s="7">
         <v>3.1</v>
       </c>
-      <c r="L18" s="15" t="s">
+      <c r="L18" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="M18" s="22">
+      <c r="M18" s="20">
         <f>AVERAGE(1,2)</f>
         <v>1.5</v>
       </c>
-      <c r="N18" s="9" t="s">
+      <c r="N18" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="O18" s="9">
+      <c r="O18" s="7">
         <f>AVERAGE(20,35)</f>
         <v>27.5</v>
       </c>
-      <c r="P18" s="9" t="s">
+      <c r="P18" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Q18" s="10">
+      <c r="Q18" s="8">
         <f>AVERAGE(80,150)</f>
         <v>115</v>
       </c>
-      <c r="R18" s="9">
+      <c r="R18" s="7">
         <v>13</v>
       </c>
-      <c r="S18" s="9">
-        <v>3</v>
-      </c>
-      <c r="T18" s="23">
+      <c r="S18" s="7">
+        <v>3</v>
+      </c>
+      <c r="T18" s="21">
         <v>2</v>
       </c>
     </row>
@@ -2360,66 +2360,66 @@
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F19" s="9">
+      <c r="E19" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="7">
         <f>AVERAGE(60,100)</f>
         <v>80</v>
       </c>
-      <c r="G19" s="9">
-        <v>3</v>
-      </c>
-      <c r="H19" s="9">
-        <v>3</v>
-      </c>
-      <c r="I19" s="15" t="s">
+      <c r="G19" s="7">
+        <v>3</v>
+      </c>
+      <c r="H19" s="7">
+        <v>3</v>
+      </c>
+      <c r="I19" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="J19" s="9">
+      <c r="J19" s="7">
         <f>AVERAGE(10,15)</f>
         <v>12.5</v>
       </c>
-      <c r="K19" s="9">
+      <c r="K19" s="7">
         <v>1.9</v>
       </c>
-      <c r="L19" s="15" t="s">
+      <c r="L19" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="M19" s="22">
+      <c r="M19" s="20">
         <f t="shared" ref="M19:M20" si="6">AVERAGE(2,4)</f>
         <v>3</v>
       </c>
-      <c r="N19" s="9" t="s">
+      <c r="N19" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="O19" s="9">
+      <c r="O19" s="7">
         <f>AVERAGE(30,45)</f>
         <v>37.5</v>
       </c>
-      <c r="P19" s="10" t="s">
+      <c r="P19" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="Q19" s="10">
+      <c r="Q19" s="8">
         <f>AVERAGE(150,250)</f>
         <v>200</v>
       </c>
-      <c r="R19" s="9">
+      <c r="R19" s="7">
         <v>38</v>
       </c>
-      <c r="S19" s="9">
-        <v>3</v>
-      </c>
-      <c r="T19" s="9">
+      <c r="S19" s="7">
+        <v>3</v>
+      </c>
+      <c r="T19" s="7">
         <v>2</v>
       </c>
     </row>
@@ -2427,66 +2427,66 @@
       <c r="A20" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="7">
         <f>AVERAGE(70,100)</f>
         <v>85</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="7">
         <v>1</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="7">
         <v>1</v>
       </c>
-      <c r="I20" s="15" t="s">
+      <c r="I20" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="J20" s="9">
+      <c r="J20" s="7">
         <f>AVERAGE(8,10)</f>
         <v>9</v>
       </c>
-      <c r="K20" s="9">
+      <c r="K20" s="7">
         <v>2.7</v>
       </c>
-      <c r="L20" s="15" t="s">
+      <c r="L20" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="M20" s="22">
+      <c r="M20" s="20">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="N20" s="9" t="s">
+      <c r="N20" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="O20" s="9">
+      <c r="O20" s="7">
         <f>AVERAGE(30,45)</f>
         <v>37.5</v>
       </c>
-      <c r="P20" s="10" t="s">
+      <c r="P20" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="Q20" s="10">
+      <c r="Q20" s="8">
         <f>AVERAGE(150,250)</f>
         <v>200</v>
       </c>
-      <c r="R20" s="9">
+      <c r="R20" s="7">
         <v>24</v>
       </c>
-      <c r="S20" s="9">
+      <c r="S20" s="7">
         <v>1</v>
       </c>
-      <c r="T20" s="9">
+      <c r="T20" s="7">
         <v>3</v>
       </c>
     </row>
@@ -2494,66 +2494,66 @@
       <c r="A21" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="7">
         <f>AVERAGE(50,80)</f>
         <v>65</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="7">
         <v>1</v>
       </c>
-      <c r="H21" s="9">
-        <v>2</v>
-      </c>
-      <c r="I21" s="15" t="s">
+      <c r="H21" s="7">
+        <v>2</v>
+      </c>
+      <c r="I21" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="J21" s="9">
+      <c r="J21" s="7">
         <f>AVERAGE(6,8)</f>
         <v>7</v>
       </c>
-      <c r="K21" s="9">
+      <c r="K21" s="7">
         <v>4.0999999999999996</v>
       </c>
-      <c r="L21" s="15" t="s">
+      <c r="L21" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="M21" s="22">
+      <c r="M21" s="20">
         <f>AVERAGE(1,2)</f>
         <v>1.5</v>
       </c>
-      <c r="N21" s="9" t="s">
+      <c r="N21" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="O21" s="9">
+      <c r="O21" s="7">
         <f>AVERAGE(20,35)</f>
         <v>27.5</v>
       </c>
-      <c r="P21" s="10" t="s">
+      <c r="P21" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="Q21" s="10">
+      <c r="Q21" s="8">
         <f>AVERAGE(80,150)</f>
         <v>115</v>
       </c>
-      <c r="R21" s="9">
+      <c r="R21" s="7">
         <v>13</v>
       </c>
-      <c r="S21" s="9">
+      <c r="S21" s="7">
         <v>1</v>
       </c>
-      <c r="T21" s="9">
+      <c r="T21" s="7">
         <v>2</v>
       </c>
     </row>
@@ -2561,66 +2561,66 @@
       <c r="A22" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="E22" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F22" s="9">
+      <c r="E22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="7">
         <f>AVERAGE(60,100)</f>
         <v>80</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="7">
         <v>1</v>
       </c>
-      <c r="H22" s="9">
+      <c r="H22" s="7">
         <v>1</v>
       </c>
-      <c r="I22" s="15" t="s">
+      <c r="I22" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="J22" s="9">
+      <c r="J22" s="7">
         <f>AVERAGE(2,4)</f>
         <v>3</v>
       </c>
-      <c r="K22" s="9">
+      <c r="K22" s="7">
         <v>2.8</v>
       </c>
-      <c r="L22" s="15" t="s">
+      <c r="L22" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="M22" s="22">
+      <c r="M22" s="20">
         <f>AVERAGE(1,2)</f>
         <v>1.5</v>
       </c>
-      <c r="N22" s="9" t="s">
+      <c r="N22" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="O22" s="9">
+      <c r="O22" s="7">
         <f>AVERAGE(20,35)</f>
         <v>27.5</v>
       </c>
-      <c r="P22" s="9" t="s">
+      <c r="P22" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Q22" s="10">
+      <c r="Q22" s="8">
         <f>AVERAGE(80,150)</f>
         <v>115</v>
       </c>
-      <c r="R22" s="9">
+      <c r="R22" s="7">
         <v>6</v>
       </c>
-      <c r="S22" s="9">
+      <c r="S22" s="7">
         <v>1</v>
       </c>
-      <c r="T22" s="9">
+      <c r="T22" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2628,66 +2628,66 @@
       <c r="A23" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="E23" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F23" s="9">
+      <c r="E23" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" s="7">
         <f>AVERAGE(60,100)</f>
         <v>80</v>
       </c>
-      <c r="G23" s="9">
-        <v>3</v>
-      </c>
-      <c r="H23" s="9">
-        <v>3</v>
-      </c>
-      <c r="I23" s="15" t="s">
+      <c r="G23" s="7">
+        <v>3</v>
+      </c>
+      <c r="H23" s="7">
+        <v>3</v>
+      </c>
+      <c r="I23" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="J23" s="9">
+      <c r="J23" s="7">
         <f>AVERAGE(8,12)</f>
         <v>10</v>
       </c>
-      <c r="K23" s="9">
+      <c r="K23" s="7">
         <v>2.4</v>
       </c>
-      <c r="L23" s="15" t="s">
+      <c r="L23" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="M23" s="22">
+      <c r="M23" s="20">
         <f t="shared" ref="M23" si="7">AVERAGE(2,4)</f>
         <v>3</v>
       </c>
-      <c r="N23" s="9" t="s">
+      <c r="N23" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="O23" s="9">
+      <c r="O23" s="7">
         <f>AVERAGE(30,45)</f>
         <v>37.5</v>
       </c>
-      <c r="P23" s="9" t="s">
+      <c r="P23" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="Q23" s="10">
+      <c r="Q23" s="8">
         <f>AVERAGE(150,250)</f>
         <v>200</v>
       </c>
-      <c r="R23" s="9">
+      <c r="R23" s="7">
         <v>24</v>
       </c>
-      <c r="S23" s="9">
-        <v>3</v>
-      </c>
-      <c r="T23" s="23">
+      <c r="S23" s="7">
+        <v>3</v>
+      </c>
+      <c r="T23" s="21">
         <v>2</v>
       </c>
     </row>
@@ -2695,66 +2695,66 @@
       <c r="A24" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24" s="7">
         <f>AVERAGE(40,60)</f>
         <v>50</v>
       </c>
-      <c r="G24" s="9">
-        <v>2</v>
-      </c>
-      <c r="H24" s="9">
-        <v>2</v>
-      </c>
-      <c r="I24" s="15" t="s">
+      <c r="G24" s="7">
+        <v>2</v>
+      </c>
+      <c r="H24" s="7">
+        <v>2</v>
+      </c>
+      <c r="I24" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="J24" s="9">
+      <c r="J24" s="7">
         <f>AVERAGE(3,5)</f>
         <v>4</v>
       </c>
-      <c r="K24" s="9">
+      <c r="K24" s="7">
         <v>4.5</v>
       </c>
-      <c r="L24" s="15" t="s">
+      <c r="L24" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="M24" s="22">
+      <c r="M24" s="20">
         <f>AVERAGE(1,2)</f>
         <v>1.5</v>
       </c>
-      <c r="N24" s="9" t="s">
+      <c r="N24" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="O24" s="9">
+      <c r="O24" s="7">
         <f>AVERAGE(20,35)</f>
         <v>27.5</v>
       </c>
-      <c r="P24" s="9" t="s">
+      <c r="P24" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Q24" s="10">
+      <c r="Q24" s="8">
         <f>AVERAGE(80,150)</f>
         <v>115</v>
       </c>
-      <c r="R24" s="9">
-        <v>13</v>
-      </c>
-      <c r="S24" s="9">
-        <v>3</v>
-      </c>
-      <c r="T24" s="23">
+      <c r="R24" s="7">
+        <v>6</v>
+      </c>
+      <c r="S24" s="7">
+        <v>3</v>
+      </c>
+      <c r="T24" s="21">
         <v>1</v>
       </c>
     </row>
@@ -2762,66 +2762,66 @@
       <c r="A25" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D25" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E25" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F25" s="9">
+      <c r="E25" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="7">
         <f>AVERAGE(60,100)</f>
         <v>80</v>
       </c>
-      <c r="G25" s="9">
-        <v>2</v>
-      </c>
-      <c r="H25" s="9">
+      <c r="G25" s="7">
+        <v>2</v>
+      </c>
+      <c r="H25" s="7">
         <v>1</v>
       </c>
-      <c r="I25" s="15" t="s">
+      <c r="I25" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="J25" s="9">
+      <c r="J25" s="7">
         <f>AVERAGE(3,5)</f>
         <v>4</v>
       </c>
-      <c r="K25" s="9">
+      <c r="K25" s="7">
         <v>4</v>
       </c>
-      <c r="L25" s="15" t="s">
+      <c r="L25" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="M25" s="22">
+      <c r="M25" s="20">
         <f>AVERAGE(1,2)</f>
         <v>1.5</v>
       </c>
-      <c r="N25" s="9" t="s">
+      <c r="N25" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="O25" s="9">
+      <c r="O25" s="7">
         <f>AVERAGE(20,35)</f>
         <v>27.5</v>
       </c>
-      <c r="P25" s="9" t="s">
+      <c r="P25" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Q25" s="10">
+      <c r="Q25" s="8">
         <f>AVERAGE(80,150)</f>
         <v>115</v>
       </c>
-      <c r="R25" s="9">
-        <v>3</v>
-      </c>
-      <c r="S25" s="9">
-        <v>3</v>
-      </c>
-      <c r="T25" s="23">
+      <c r="R25" s="7">
+        <v>6</v>
+      </c>
+      <c r="S25" s="7">
+        <v>3</v>
+      </c>
+      <c r="T25" s="21">
         <v>3</v>
       </c>
     </row>
@@ -2829,198 +2829,198 @@
       <c r="A26" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="D26" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="E26" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F26" s="9">
+      <c r="F26" s="7">
         <f>AVERAGE(50,80)</f>
         <v>65</v>
       </c>
-      <c r="G26" s="9">
-        <v>2</v>
-      </c>
-      <c r="H26" s="9">
-        <v>2</v>
-      </c>
-      <c r="I26" s="15" t="s">
+      <c r="G26" s="7">
+        <v>2</v>
+      </c>
+      <c r="H26" s="7">
+        <v>2</v>
+      </c>
+      <c r="I26" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="J26" s="9">
+      <c r="J26" s="7">
         <f>AVERAGE(3,5)</f>
         <v>4</v>
       </c>
-      <c r="K26" s="9">
-        <v>2</v>
-      </c>
-      <c r="L26" s="15" t="s">
+      <c r="K26" s="7">
+        <v>2</v>
+      </c>
+      <c r="L26" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="M26" s="22">
+      <c r="M26" s="20">
         <f>AVERAGE(1,2)</f>
         <v>1.5</v>
       </c>
-      <c r="N26" s="9" t="s">
+      <c r="N26" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="O26" s="9">
+      <c r="O26" s="7">
         <f>AVERAGE(20,35)</f>
         <v>27.5</v>
       </c>
-      <c r="P26" s="9" t="s">
+      <c r="P26" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Q26" s="10">
+      <c r="Q26" s="8">
         <f>AVERAGE(80,150)</f>
         <v>115</v>
       </c>
-      <c r="R26" s="9">
-        <v>13</v>
-      </c>
-      <c r="S26" s="9">
-        <v>3</v>
-      </c>
-      <c r="T26" s="23">
+      <c r="R26" s="7">
+        <v>6</v>
+      </c>
+      <c r="S26" s="7">
+        <v>3</v>
+      </c>
+      <c r="T26" s="21">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="85" customHeight="1">
-      <c r="A29" s="16"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
+      <c r="A29" s="14"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
     </row>
     <row r="30" spans="1:20" ht="105" customHeight="1">
-      <c r="A30" s="14"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
+      <c r="A30" s="12"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
     </row>
     <row r="31" spans="1:20" ht="260" customHeight="1">
-      <c r="A31" s="14"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
     </row>
     <row r="32" spans="1:20" ht="13">
-      <c r="A32" s="14"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
     </row>
     <row r="33" spans="1:8" ht="112" customHeight="1">
-      <c r="A33" s="14"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
+      <c r="A33" s="12"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
     </row>
     <row r="34" spans="1:8" ht="104" customHeight="1">
-      <c r="A34" s="14"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
+      <c r="A34" s="12"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
     </row>
     <row r="35" spans="1:8" ht="178.5" customHeight="1">
-      <c r="A35" s="14"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
+      <c r="A35" s="12"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
     </row>
     <row r="36" spans="1:8" ht="166" customHeight="1">
-      <c r="A36" s="14"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
+      <c r="A36" s="12"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
     </row>
     <row r="37" spans="1:8" ht="264.5" customHeight="1">
-      <c r="A37" s="14"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
+      <c r="A37" s="12"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
     </row>
     <row r="38" spans="1:8" ht="97" customHeight="1">
-      <c r="A38" s="14"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
     </row>
     <row r="39" spans="1:8" ht="13">
-      <c r="A39" s="14"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
     </row>
     <row r="40" spans="1:8" ht="320.5" customHeight="1">
-      <c r="A40" s="14"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
     </row>
     <row r="41" spans="1:8" ht="13">
-      <c r="A41" s="14"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
+      <c r="A41" s="12"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
     </row>
     <row r="44" spans="1:8" ht="13">
-      <c r="A44" s="11"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
+      <c r="A44" s="9"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
     </row>
     <row r="45" spans="1:8" ht="40.5" customHeight="1">
-      <c r="A45" s="12"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
+      <c r="A45" s="10"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
     </row>
     <row r="46" spans="1:8" ht="55.5" customHeight="1">
-      <c r="A46" s="12"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
+      <c r="A46" s="10"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
     </row>
     <row r="47" spans="1:8" ht="41.5" customHeight="1">
-      <c r="A47" s="12"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
+      <c r="A47" s="10"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
     </row>
     <row r="50" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A50" s="6"/>
+      <c r="A50" s="4"/>
     </row>
     <row r="52" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A52" s="6"/>
+      <c r="A52" s="4"/>
     </row>
     <row r="54" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A54" s="6"/>
+      <c r="A54" s="4"/>
     </row>
     <row r="56" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A56" s="6"/>
+      <c r="A56" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -3038,8 +3038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D94A6515-3C09-47CC-B0A5-2DE33CEBC81B}">
   <dimension ref="A2:B13"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5"/>
@@ -3049,98 +3049,98 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" ht="136" customHeight="1">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="11" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="148" customHeight="1">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="11" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="315" customHeight="1">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="366.5" customHeight="1">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="11" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="141" customHeight="1">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="157.5" customHeight="1">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="11" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="231" customHeight="1">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="243" customHeight="1">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="11" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="321.5" customHeight="1">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="11" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="155" customHeight="1">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="328.5" customHeight="1">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="11" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="409.5">
-      <c r="A13" s="14" t="s">
+    <row r="13" spans="1:2" ht="400">
+      <c r="A13" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="18" t="s">
         <v>125</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add code for top 3 Belaege
</commit_message>
<xml_diff>
--- a/00_data_raw/Rohdaten_Matrix_Baeume.xlsx
+++ b/00_data_raw/Rohdaten_Matrix_Baeume.xlsx
@@ -1127,8 +1127,8 @@
   </sheetPr>
   <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H14" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2:R26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Add new analysis plot for rohdaten bäume und beläge
</commit_message>
<xml_diff>
--- a/00_data_raw/Rohdaten_Matrix_Baeume.xlsx
+++ b/00_data_raw/Rohdaten_Matrix_Baeume.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zhaw-my.sharepoint.com/personal/pfeifsar_students_zhaw_ch/Documents/6. Semester MSc UnR/Thesis/R_Project/00_data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="705" documentId="13_ncr:1_{F5B91F4B-6C5E-40FC-8FE7-21E477E3C12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7437B8A8-37BF-490F-9BAC-E28D7CE902F4}"/>
+  <xr:revisionPtr revIDLastSave="708" documentId="13_ncr:1_{F5B91F4B-6C5E-40FC-8FE7-21E477E3C12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCD1DB6E-EDA4-461E-BAC7-2589A1995818}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="127">
   <si>
     <t>Baumkategorie</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Lebensdauer in Städte [a]</t>
-  </si>
-  <si>
-    <t>120-250</t>
   </si>
   <si>
     <t>80-150</t>
@@ -1127,8 +1124,8 @@
   </sheetPr>
   <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1163,72 +1160,72 @@
         <v>1</v>
       </c>
       <c r="C1" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="22" t="s">
         <v>46</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>47</v>
       </c>
       <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H1" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="I1" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="22" t="s">
+      <c r="K1" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="K1" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" s="22" t="s">
+      <c r="M1" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="M1" s="22" t="s">
+      <c r="N1" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="N1" s="22" t="s">
+      <c r="O1" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="P1" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="O1" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="P1" s="22" t="s">
+      <c r="Q1" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="22" t="s">
+      <c r="R1" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="S1" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="R1" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="S1" s="22" t="s">
-        <v>117</v>
-      </c>
       <c r="T1" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>2</v>
@@ -1244,7 +1241,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J2" s="7">
         <f>AVERAGE(15,20)</f>
@@ -1254,7 +1251,7 @@
         <v>4.7</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M2" s="20">
         <f>AVERAGE(4,6)</f>
@@ -1268,7 +1265,7 @@
         <v>50</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q2" s="8">
         <f>AVERAGE(250,400)</f>
@@ -1286,16 +1283,16 @@
     </row>
     <row r="3" spans="1:20" ht="15.5" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>2</v>
@@ -1311,7 +1308,7 @@
         <v>2</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J3" s="7">
         <f t="shared" ref="J3:J4" si="0">AVERAGE(15,20)</f>
@@ -1321,7 +1318,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M3" s="20">
         <f t="shared" ref="M3:M7" si="1">AVERAGE(4,6)</f>
@@ -1335,7 +1332,7 @@
         <v>50</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q3" s="8">
         <f t="shared" ref="Q3:Q7" si="3">AVERAGE(250,400)</f>
@@ -1353,19 +1350,19 @@
     </row>
     <row r="4" spans="1:20" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" s="7">
         <f>AVERAGE(70,90)</f>
@@ -1378,7 +1375,7 @@
         <v>3</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J4" s="7">
         <f t="shared" si="0"/>
@@ -1388,7 +1385,7 @@
         <v>3.6</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M4" s="20">
         <f t="shared" si="1"/>
@@ -1402,7 +1399,7 @@
         <v>50</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q4" s="8">
         <f t="shared" si="3"/>
@@ -1420,16 +1417,16 @@
     </row>
     <row r="5" spans="1:20" ht="15.5" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>3</v>
@@ -1445,7 +1442,7 @@
         <v>3</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J5" s="7">
         <f>AVERAGE(12,15)</f>
@@ -1455,21 +1452,21 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="L5" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M5" s="20">
         <f>AVERAGE(2,4)</f>
         <v>3</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O5" s="7">
         <f>AVERAGE(30,45)</f>
         <v>37.5</v>
       </c>
       <c r="P5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q5" s="8">
         <f>AVERAGE(150,250)</f>
@@ -1487,16 +1484,16 @@
     </row>
     <row r="6" spans="1:20" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>2</v>
@@ -1512,7 +1509,7 @@
         <v>3</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J6" s="7">
         <f>AVERAGE(12,18)</f>
@@ -1522,7 +1519,7 @@
         <v>4</v>
       </c>
       <c r="L6" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M6" s="20">
         <f t="shared" si="1"/>
@@ -1536,7 +1533,7 @@
         <v>50</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q6" s="8">
         <f t="shared" si="3"/>
@@ -1554,16 +1551,16 @@
     </row>
     <row r="7" spans="1:20" ht="14.5">
       <c r="A7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C7" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="17" t="s">
         <v>48</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>49</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>3</v>
@@ -1579,7 +1576,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J7" s="7">
         <f>AVERAGE(12,18)</f>
@@ -1589,7 +1586,7 @@
         <v>2</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M7" s="20">
         <f t="shared" si="1"/>
@@ -1603,7 +1600,7 @@
         <v>50</v>
       </c>
       <c r="P7" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q7" s="8">
         <f t="shared" si="3"/>
@@ -1621,19 +1618,19 @@
     </row>
     <row r="8" spans="1:20" ht="15.5" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" s="7">
         <f>AVERAGE(60,80)</f>
@@ -1646,7 +1643,7 @@
         <v>1</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J8" s="7">
         <f>AVERAGE(8,10)</f>
@@ -1656,25 +1653,25 @@
         <v>1.4</v>
       </c>
       <c r="L8" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M8" s="20">
         <f>AVERAGE(2,4)</f>
         <v>3</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O8" s="7">
         <f>AVERAGE(30,45)</f>
         <v>37.5</v>
       </c>
       <c r="P8" s="8" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="Q8" s="8">
-        <f>AVERAGE(120,250)</f>
-        <v>185</v>
+        <f>AVERAGE(150,250)</f>
+        <v>200</v>
       </c>
       <c r="R8" s="7">
         <v>24</v>
@@ -1688,19 +1685,19 @@
     </row>
     <row r="9" spans="1:20" ht="15.5" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C9" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="17" t="s">
-        <v>51</v>
-      </c>
       <c r="E9" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F9" s="7">
         <f>AVERAGE(60,90)</f>
@@ -1713,7 +1710,7 @@
         <v>2</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J9" s="7">
         <f>AVERAGE(5,8)</f>
@@ -1723,21 +1720,21 @@
         <v>3</v>
       </c>
       <c r="L9" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M9" s="20">
         <f t="shared" ref="M9:M16" si="4">AVERAGE(2,4)</f>
         <v>3</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O9" s="7">
         <f>AVERAGE(30,45)</f>
         <v>37.5</v>
       </c>
       <c r="P9" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q9" s="8">
         <f>AVERAGE(150,250)</f>
@@ -1755,16 +1752,16 @@
     </row>
     <row r="10" spans="1:20" ht="15.5" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="17" t="s">
         <v>53</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>54</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>2</v>
@@ -1780,7 +1777,7 @@
         <v>3</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J10" s="7">
         <f>AVERAGE(10,15)</f>
@@ -1790,21 +1787,21 @@
         <v>2.5</v>
       </c>
       <c r="L10" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M10" s="20">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O10" s="7">
         <f>AVERAGE(30,45)</f>
         <v>37.5</v>
       </c>
       <c r="P10" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q10" s="8">
         <f>AVERAGE(150,250)</f>
@@ -1822,16 +1819,16 @@
     </row>
     <row r="11" spans="1:20" ht="15.5" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>3</v>
@@ -1847,7 +1844,7 @@
         <v>2</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J11" s="7">
         <f>AVERAGE(8,12)</f>
@@ -1857,21 +1854,21 @@
         <v>2.4</v>
       </c>
       <c r="L11" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M11" s="20">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O11" s="7">
         <f>AVERAGE(30,45)</f>
         <v>37.5</v>
       </c>
       <c r="P11" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q11" s="8">
         <f>AVERAGE(150,250)</f>
@@ -1889,16 +1886,16 @@
     </row>
     <row r="12" spans="1:20" ht="15.5" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="17" t="s">
         <v>56</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>57</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>3</v>
@@ -1914,7 +1911,7 @@
         <v>2</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J12" s="7">
         <f>AVERAGE(6,10)</f>
@@ -1924,21 +1921,21 @@
         <v>2</v>
       </c>
       <c r="L12" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M12" s="20">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="N12" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O12" s="7">
         <f>AVERAGE(30,45)</f>
         <v>37.5</v>
       </c>
       <c r="P12" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q12" s="8">
         <f>AVERAGE(150,250)</f>
@@ -1956,16 +1953,16 @@
     </row>
     <row r="13" spans="1:20" ht="15" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>2</v>
@@ -1981,7 +1978,7 @@
         <v>3</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J13" s="7">
         <f>AVERAGE(5,6)</f>
@@ -1991,21 +1988,21 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="L13" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M13" s="20">
         <f>AVERAGE(1,2)</f>
         <v>1.5</v>
       </c>
       <c r="N13" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O13" s="7">
         <f>AVERAGE(20,35)</f>
         <v>27.5</v>
       </c>
       <c r="P13" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q13" s="8">
         <f>AVERAGE(80,150)</f>
@@ -2023,16 +2020,16 @@
     </row>
     <row r="14" spans="1:20" ht="15.75" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>3</v>
@@ -2048,7 +2045,7 @@
         <v>3</v>
       </c>
       <c r="I14" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J14" s="7">
         <f>AVERAGE(4,6)</f>
@@ -2058,21 +2055,21 @@
         <v>4.3</v>
       </c>
       <c r="L14" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M14" s="20">
         <f>AVERAGE(1,2)</f>
         <v>1.5</v>
       </c>
       <c r="N14" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O14" s="7">
         <f>AVERAGE(20,35)</f>
         <v>27.5</v>
       </c>
       <c r="P14" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q14" s="8">
         <f>AVERAGE(80,150)</f>
@@ -2090,19 +2087,19 @@
     </row>
     <row r="15" spans="1:20" ht="15.75" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" s="7">
         <f>AVERAGE(70,100)</f>
@@ -2115,7 +2112,7 @@
         <v>2</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J15" s="7">
         <f>AVERAGE(10,15)</f>
@@ -2125,21 +2122,21 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="L15" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M15" s="20">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O15" s="7">
         <f>AVERAGE(30,45)</f>
         <v>37.5</v>
       </c>
       <c r="P15" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q15" s="8">
         <f>AVERAGE(150,250)</f>
@@ -2157,16 +2154,16 @@
     </row>
     <row r="16" spans="1:20" ht="15.75" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>3</v>
@@ -2182,7 +2179,7 @@
         <v>3</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J16" s="7">
         <f>AVERAGE(8,12)</f>
@@ -2192,21 +2189,21 @@
         <v>2.4</v>
       </c>
       <c r="L16" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M16" s="20">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="N16" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O16" s="7">
         <f>AVERAGE(30,45)</f>
         <v>37.5</v>
       </c>
       <c r="P16" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q16" s="8">
         <f>AVERAGE(150,250)</f>
@@ -2224,19 +2221,19 @@
     </row>
     <row r="17" spans="1:20" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F17" s="7">
         <f>AVERAGE(60,90)</f>
@@ -2249,7 +2246,7 @@
         <v>3</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J17" s="7">
         <f>AVERAGE(4,7)</f>
@@ -2259,21 +2256,21 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="L17" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M17" s="20">
         <f>AVERAGE(1,2)</f>
         <v>1.5</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O17" s="7">
         <f>AVERAGE(20,35)</f>
         <v>27.5</v>
       </c>
       <c r="P17" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q17" s="8">
         <f>AVERAGE(80,150)</f>
@@ -2291,19 +2288,19 @@
     </row>
     <row r="18" spans="1:20" ht="13">
       <c r="A18" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F18" s="7">
         <f>AVERAGE(70,100)</f>
@@ -2316,7 +2313,7 @@
         <v>2</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J18" s="7">
         <f>AVERAGE(4,6)</f>
@@ -2326,21 +2323,21 @@
         <v>3.1</v>
       </c>
       <c r="L18" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M18" s="20">
         <f>AVERAGE(1,2)</f>
         <v>1.5</v>
       </c>
       <c r="N18" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O18" s="7">
         <f>AVERAGE(20,35)</f>
         <v>27.5</v>
       </c>
       <c r="P18" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q18" s="8">
         <f>AVERAGE(80,150)</f>
@@ -2358,16 +2355,16 @@
     </row>
     <row r="19" spans="1:20" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>3</v>
@@ -2383,7 +2380,7 @@
         <v>3</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J19" s="7">
         <f>AVERAGE(10,15)</f>
@@ -2393,21 +2390,21 @@
         <v>1.9</v>
       </c>
       <c r="L19" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M19" s="20">
         <f t="shared" ref="M19:M20" si="6">AVERAGE(2,4)</f>
         <v>3</v>
       </c>
       <c r="N19" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O19" s="7">
         <f>AVERAGE(30,45)</f>
         <v>37.5</v>
       </c>
       <c r="P19" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q19" s="8">
         <f>AVERAGE(150,250)</f>
@@ -2425,19 +2422,19 @@
     </row>
     <row r="20" spans="1:20" ht="15.75" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F20" s="7">
         <f>AVERAGE(70,100)</f>
@@ -2450,7 +2447,7 @@
         <v>1</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J20" s="7">
         <f>AVERAGE(8,10)</f>
@@ -2460,21 +2457,21 @@
         <v>2.7</v>
       </c>
       <c r="L20" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M20" s="20">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="N20" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O20" s="7">
         <f>AVERAGE(30,45)</f>
         <v>37.5</v>
       </c>
       <c r="P20" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q20" s="8">
         <f>AVERAGE(150,250)</f>
@@ -2492,19 +2489,19 @@
     </row>
     <row r="21" spans="1:20" ht="15.75" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" s="7">
         <f>AVERAGE(50,80)</f>
@@ -2517,7 +2514,7 @@
         <v>2</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J21" s="7">
         <f>AVERAGE(6,8)</f>
@@ -2527,21 +2524,21 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="L21" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M21" s="20">
         <f>AVERAGE(1,2)</f>
         <v>1.5</v>
       </c>
       <c r="N21" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O21" s="7">
         <f>AVERAGE(20,35)</f>
         <v>27.5</v>
       </c>
       <c r="P21" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q21" s="8">
         <f>AVERAGE(80,150)</f>
@@ -2559,16 +2556,16 @@
     </row>
     <row r="22" spans="1:20" ht="15.75" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>3</v>
@@ -2584,7 +2581,7 @@
         <v>1</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J22" s="7">
         <f>AVERAGE(2,4)</f>
@@ -2594,21 +2591,21 @@
         <v>2.8</v>
       </c>
       <c r="L22" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M22" s="20">
         <f>AVERAGE(1,2)</f>
         <v>1.5</v>
       </c>
       <c r="N22" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O22" s="7">
         <f>AVERAGE(20,35)</f>
         <v>27.5</v>
       </c>
       <c r="P22" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q22" s="8">
         <f>AVERAGE(80,150)</f>
@@ -2626,16 +2623,16 @@
     </row>
     <row r="23" spans="1:20" ht="15.75" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>3</v>
@@ -2651,7 +2648,7 @@
         <v>3</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J23" s="7">
         <f>AVERAGE(8,12)</f>
@@ -2661,21 +2658,21 @@
         <v>2.4</v>
       </c>
       <c r="L23" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M23" s="20">
         <f t="shared" ref="M23" si="7">AVERAGE(2,4)</f>
         <v>3</v>
       </c>
       <c r="N23" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O23" s="7">
         <f>AVERAGE(30,45)</f>
         <v>37.5</v>
       </c>
       <c r="P23" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q23" s="8">
         <f>AVERAGE(150,250)</f>
@@ -2693,19 +2690,19 @@
     </row>
     <row r="24" spans="1:20" ht="15.75" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C24" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="17" t="s">
-        <v>61</v>
-      </c>
       <c r="E24" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F24" s="7">
         <f>AVERAGE(40,60)</f>
@@ -2718,7 +2715,7 @@
         <v>2</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J24" s="7">
         <f>AVERAGE(3,5)</f>
@@ -2728,21 +2725,21 @@
         <v>4.5</v>
       </c>
       <c r="L24" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M24" s="20">
         <f>AVERAGE(1,2)</f>
         <v>1.5</v>
       </c>
       <c r="N24" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O24" s="7">
         <f>AVERAGE(20,35)</f>
         <v>27.5</v>
       </c>
       <c r="P24" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q24" s="8">
         <f>AVERAGE(80,150)</f>
@@ -2760,16 +2757,16 @@
     </row>
     <row r="25" spans="1:20" ht="15.75" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C25" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="17" t="s">
         <v>63</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>64</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>3</v>
@@ -2785,7 +2782,7 @@
         <v>1</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J25" s="7">
         <f>AVERAGE(3,5)</f>
@@ -2795,21 +2792,21 @@
         <v>4</v>
       </c>
       <c r="L25" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M25" s="20">
         <f>AVERAGE(1,2)</f>
         <v>1.5</v>
       </c>
       <c r="N25" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O25" s="7">
         <f>AVERAGE(20,35)</f>
         <v>27.5</v>
       </c>
       <c r="P25" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q25" s="8">
         <f>AVERAGE(80,150)</f>
@@ -2827,19 +2824,19 @@
     </row>
     <row r="26" spans="1:20" ht="15.75" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26" s="7">
         <f>AVERAGE(50,80)</f>
@@ -2852,7 +2849,7 @@
         <v>2</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J26" s="7">
         <f>AVERAGE(3,5)</f>
@@ -2862,21 +2859,21 @@
         <v>2</v>
       </c>
       <c r="L26" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M26" s="20">
         <f>AVERAGE(1,2)</f>
         <v>1.5</v>
       </c>
       <c r="N26" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O26" s="7">
         <f>AVERAGE(20,35)</f>
         <v>27.5</v>
       </c>
       <c r="P26" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q26" s="8">
         <f>AVERAGE(80,150)</f>
@@ -3038,7 +3035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D94A6515-3C09-47CC-B0A5-2DE33CEBC81B}">
   <dimension ref="A2:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
@@ -3050,98 +3047,98 @@
   <sheetData>
     <row r="2" spans="1:2" ht="136" customHeight="1">
       <c r="A2" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="148" customHeight="1">
       <c r="A3" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="315" customHeight="1">
       <c r="A4" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="366.5" customHeight="1">
       <c r="A5" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="141" customHeight="1">
       <c r="A6" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="157.5" customHeight="1">
       <c r="A7" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="231" customHeight="1">
       <c r="A8" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="243" customHeight="1">
       <c r="A9" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="321.5" customHeight="1">
       <c r="A10" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="155" customHeight="1">
       <c r="A11" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="328.5" customHeight="1">
       <c r="A12" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="400">
       <c r="A13" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix umbenennung umweltbelastung zu umweltwirkung
</commit_message>
<xml_diff>
--- a/00_data_raw/Rohdaten_Matrix_Baeume.xlsx
+++ b/00_data_raw/Rohdaten_Matrix_Baeume.xlsx
@@ -1124,8 +1124,8 @@
   </sheetPr>
   <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>